<commit_message>
Making changes for Data_Meghana
Making changes for Data_Meghana
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/Pre-Release/Data_Meghana.xlsx
+++ b/svmx/test_lab/test_cases/analytics/Pre-Release/Data_Meghana.xlsx
@@ -56,9 +56,6 @@
     <t>System.Today()</t>
   </si>
   <si>
-    <t>a1Zq0000001jyS9</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
@@ -183,6 +180,9 @@
   </si>
   <si>
     <t>a0T1g0000008TIjEAM</t>
+  </si>
+  <si>
+    <t>a2N1g000000EWRz</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,16 +720,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -738,63 +738,63 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="P1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="R1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="W1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="Y1" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -803,31 +803,31 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="N2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="P2" s="1">
         <v>30</v>
@@ -836,19 +836,19 @@
         <v>43121</v>
       </c>
       <c r="R2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="T2" s="1">
         <v>44640</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W2" s="1">
         <v>360</v>
@@ -857,30 +857,30 @@
         <v>98.33</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C3" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Adding changes to Pre-Release test-cases
Adding changes to Pre-Release test-cases
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/Pre-Release/Data_Meghana.xlsx
+++ b/svmx/test_lab/test_cases/analytics/Pre-Release/Data_Meghana.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Account</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>a2N1g000000EWRz</t>
+  </si>
+  <si>
+    <t>ProductWarranty</t>
+  </si>
+  <si>
+    <t>a2K1g000000CgAT</t>
   </si>
 </sst>
 </file>
@@ -672,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -703,10 +709,11 @@
     <col min="23" max="23" width="28.33203125" style="1" customWidth="1"/>
     <col min="24" max="24" width="25.33203125" style="1" customWidth="1"/>
     <col min="25" max="25" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="10.83203125" style="1"/>
+    <col min="26" max="26" width="28" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -782,8 +789,11 @@
       <c r="Y1" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="Z1" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -859,8 +869,11 @@
       <c r="Y2" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="Z2" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
@@ -883,10 +896,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C5" s="10"/>
     </row>
   </sheetData>

</xml_diff>